<commit_message>
CRUD backend done Frontend: view, edit and delete done
</commit_message>
<xml_diff>
--- a/food_app/data/booking_data.xlsx
+++ b/food_app/data/booking_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jolene\Downloads\Year 1.3\DB\assg\food_app\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C614AF0-D725-4D9F-A3A2-2CD492708C6B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2AA7C64-C5F4-49B0-9118-FDF94CAB5AD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>cid</t>
   </si>
@@ -105,123 +105,6 @@
   </si>
   <si>
     <t xml:space="preserve">engagement party </t>
-  </si>
-  <si>
-    <t>9:15pm</t>
-  </si>
-  <si>
-    <t>7:45pm</t>
-  </si>
-  <si>
-    <t>6:30pm</t>
-  </si>
-  <si>
-    <t>3:15pm</t>
-  </si>
-  <si>
-    <t>12:00pm</t>
-  </si>
-  <si>
-    <t>1:05pm</t>
-  </si>
-  <si>
-    <t>9:00am</t>
-  </si>
-  <si>
-    <t>10:15am</t>
-  </si>
-  <si>
-    <t>7:15pm</t>
-  </si>
-  <si>
-    <t>5:45pm</t>
-  </si>
-  <si>
-    <t>11:55am</t>
-  </si>
-  <si>
-    <t>11:15am</t>
-  </si>
-  <si>
-    <t>6:35pm</t>
-  </si>
-  <si>
-    <t>8:10pm</t>
-  </si>
-  <si>
-    <t>2:45pm</t>
-  </si>
-  <si>
-    <t>4:35pm</t>
-  </si>
-  <si>
-    <t>12:15pm</t>
-  </si>
-  <si>
-    <t>5:30pm</t>
-  </si>
-  <si>
-    <t>8:25pm</t>
-  </si>
-  <si>
-    <t>1:45pm</t>
-  </si>
-  <si>
-    <t>6:15pm</t>
-  </si>
-  <si>
-    <t>11:45am</t>
-  </si>
-  <si>
-    <t>7:00pm</t>
-  </si>
-  <si>
-    <t>2:35pm</t>
-  </si>
-  <si>
-    <t>7:35pm</t>
-  </si>
-  <si>
-    <t>3:05pm</t>
-  </si>
-  <si>
-    <t>1:55pm</t>
-  </si>
-  <si>
-    <t>12:30pm</t>
-  </si>
-  <si>
-    <t>10:35am</t>
-  </si>
-  <si>
-    <t>6:45pm</t>
-  </si>
-  <si>
-    <t>3:20pm</t>
-  </si>
-  <si>
-    <t>2:30pm</t>
-  </si>
-  <si>
-    <t>6:10pm</t>
-  </si>
-  <si>
-    <t>10:20am</t>
-  </si>
-  <si>
-    <t>6:00pm</t>
-  </si>
-  <si>
-    <t>3:00pm</t>
-  </si>
-  <si>
-    <t>11:30am</t>
-  </si>
-  <si>
-    <t>4:45pm</t>
-  </si>
-  <si>
-    <t>2:00pm</t>
   </si>
 </sst>
 </file>
@@ -276,12 +159,6 @@
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -290,6 +167,10 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -597,19 +478,19 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:I52"/>
+  <dimension ref="A1:I51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="5.26171875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.20703125" customWidth="1"/>
-    <col min="3" max="3" width="11.62890625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="11.62890625" style="3" customWidth="1"/>
     <col min="4" max="4" width="6.89453125" customWidth="1"/>
-    <col min="5" max="5" width="21.47265625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21.47265625" style="6" customWidth="1"/>
     <col min="6" max="6" width="19.734375" customWidth="1"/>
     <col min="7" max="7" width="14.5234375" customWidth="1"/>
     <col min="8" max="8" width="7.20703125" customWidth="1"/>
@@ -625,7 +506,7 @@
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="D1" t="s">
@@ -651,23 +532,22 @@
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="1">
         <v>45348</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D2">
+      <c r="C2" s="4">
+        <v>0.88541666666666663</v>
+      </c>
+      <c r="D2" s="5">
         <v>5</v>
       </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="3">
+      <c r="F2" s="1">
         <v>45134</v>
       </c>
-      <c r="H2">
+      <c r="H2" s="5">
         <v>5</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="5">
         <v>7</v>
       </c>
     </row>
@@ -675,25 +555,25 @@
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="1">
         <v>45230</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="D3">
+      <c r="C3" s="4">
+        <v>0.82291666666666663</v>
+      </c>
+      <c r="D3" s="5">
         <v>2</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="3">
+      <c r="F3" s="1">
         <v>45137</v>
       </c>
-      <c r="H3">
+      <c r="H3" s="5">
         <v>18</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="5">
         <v>9</v>
       </c>
     </row>
@@ -701,23 +581,22 @@
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="1">
         <v>45377</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="D4">
+      <c r="C4" s="4">
+        <v>0.85416666666666663</v>
+      </c>
+      <c r="D4" s="5">
         <v>7</v>
       </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="3">
+      <c r="F4" s="1">
         <v>45157</v>
       </c>
-      <c r="H4">
+      <c r="H4" s="5">
         <v>23</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="5">
         <v>8</v>
       </c>
     </row>
@@ -725,26 +604,25 @@
       <c r="A5">
         <v>4</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="1">
         <v>45343</v>
       </c>
-      <c r="C5" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D5">
+      <c r="C5" s="4">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="D5" s="5">
         <v>3</v>
       </c>
-      <c r="E5" s="2"/>
-      <c r="F5" s="3">
+      <c r="F5" s="1">
         <v>45091</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="1">
         <v>45119</v>
       </c>
-      <c r="H5">
+      <c r="H5" s="5">
         <v>5</v>
       </c>
-      <c r="I5">
+      <c r="I5" s="5">
         <v>24</v>
       </c>
     </row>
@@ -752,25 +630,25 @@
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="1">
         <v>45348</v>
       </c>
-      <c r="C6" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6">
+      <c r="C6" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="D6" s="5">
         <v>4</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F6" s="3">
+      <c r="F6" s="1">
         <v>45141</v>
       </c>
-      <c r="H6">
+      <c r="H6" s="5">
         <v>21</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="5">
         <v>23</v>
       </c>
     </row>
@@ -778,23 +656,22 @@
       <c r="A7">
         <v>6</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="1">
         <v>45298</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="4">
+        <v>0.54513888888888895</v>
+      </c>
+      <c r="D7" s="5">
+        <v>1</v>
+      </c>
+      <c r="F7" s="1">
+        <v>45146</v>
+      </c>
+      <c r="H7" s="5">
         <v>29</v>
       </c>
-      <c r="D7">
-        <v>1</v>
-      </c>
-      <c r="E7" s="2"/>
-      <c r="F7" s="3">
-        <v>45146</v>
-      </c>
-      <c r="H7">
-        <v>29</v>
-      </c>
-      <c r="I7">
+      <c r="I7" s="5">
         <v>18</v>
       </c>
     </row>
@@ -802,23 +679,22 @@
       <c r="A8">
         <v>7</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="1">
         <v>45465</v>
       </c>
-      <c r="C8" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D8">
+      <c r="C8" s="4">
+        <v>0.375</v>
+      </c>
+      <c r="D8" s="5">
         <v>4</v>
       </c>
-      <c r="E8" s="2"/>
-      <c r="F8" s="3">
+      <c r="F8" s="1">
         <v>45161</v>
       </c>
-      <c r="H8">
+      <c r="H8" s="5">
         <v>25</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="5">
         <v>46</v>
       </c>
     </row>
@@ -826,25 +702,25 @@
       <c r="A9">
         <v>8</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="1">
         <v>45392</v>
       </c>
-      <c r="C9" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="D9">
+      <c r="C9" s="4">
+        <v>0.42708333333333331</v>
+      </c>
+      <c r="D9" s="5">
         <v>4</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="1">
         <v>45132</v>
       </c>
-      <c r="H9">
+      <c r="H9" s="5">
         <v>7</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="5">
         <v>4</v>
       </c>
     </row>
@@ -852,23 +728,22 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="1">
         <v>45413</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D10">
+      <c r="C10" s="4">
+        <v>0.80208333333333337</v>
+      </c>
+      <c r="D10" s="5">
         <v>5</v>
       </c>
-      <c r="E10" s="2"/>
-      <c r="F10" s="3">
+      <c r="F10" s="1">
         <v>45160</v>
       </c>
-      <c r="H10">
+      <c r="H10" s="5">
         <v>19</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="5">
         <v>29</v>
       </c>
     </row>
@@ -876,23 +751,22 @@
       <c r="A11">
         <v>10</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="1">
         <v>45492</v>
       </c>
-      <c r="C11" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D11">
+      <c r="C11" s="4">
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="D11" s="5">
         <v>6</v>
       </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="3">
+      <c r="F11" s="1">
         <v>45140</v>
       </c>
-      <c r="H11">
+      <c r="H11" s="5">
         <v>6</v>
       </c>
-      <c r="I11">
+      <c r="I11" s="5">
         <v>15</v>
       </c>
     </row>
@@ -900,23 +774,22 @@
       <c r="A12">
         <v>11</v>
       </c>
-      <c r="B12" s="3">
+      <c r="B12" s="1">
         <v>45153</v>
       </c>
-      <c r="C12" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D12">
+      <c r="C12" s="4">
+        <v>0.49652777777777773</v>
+      </c>
+      <c r="D12" s="5">
         <v>3</v>
       </c>
-      <c r="E12" s="2"/>
-      <c r="F12" s="3">
+      <c r="F12" s="1">
         <v>45140</v>
       </c>
-      <c r="H12">
+      <c r="H12" s="5">
         <v>17</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="5">
         <v>37</v>
       </c>
     </row>
@@ -924,23 +797,22 @@
       <c r="A13">
         <v>12</v>
       </c>
-      <c r="B13" s="3">
+      <c r="B13" s="1">
         <v>45240</v>
       </c>
-      <c r="C13" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D13">
+      <c r="C13" s="4">
+        <v>0.46875</v>
+      </c>
+      <c r="D13" s="5">
         <v>3</v>
       </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="3">
+      <c r="F13" s="1">
         <v>45157</v>
       </c>
-      <c r="H13">
+      <c r="H13" s="5">
         <v>14</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="5">
         <v>22</v>
       </c>
     </row>
@@ -948,25 +820,25 @@
       <c r="A14">
         <v>13</v>
       </c>
-      <c r="B14" s="3">
+      <c r="B14" s="1">
         <v>45225</v>
       </c>
-      <c r="C14" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14">
+      <c r="C14" s="4">
+        <v>0.77430555555555547</v>
+      </c>
+      <c r="D14" s="5">
         <v>2</v>
       </c>
-      <c r="E14" s="2" t="s">
+      <c r="E14" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F14" s="3">
+      <c r="F14" s="1">
         <v>45147</v>
       </c>
-      <c r="H14">
+      <c r="H14" s="5">
         <v>27</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="5">
         <v>4</v>
       </c>
     </row>
@@ -974,23 +846,22 @@
       <c r="A15">
         <v>14</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B15" s="1">
         <v>45335</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="D15">
+      <c r="C15" s="4">
+        <v>0.84027777777777779</v>
+      </c>
+      <c r="D15" s="5">
         <v>4</v>
       </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="3">
+      <c r="F15" s="1">
         <v>45146</v>
       </c>
-      <c r="H15">
+      <c r="H15" s="5">
         <v>23</v>
       </c>
-      <c r="I15">
+      <c r="I15" s="5">
         <v>36</v>
       </c>
     </row>
@@ -998,28 +869,28 @@
       <c r="A16">
         <v>15</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B16" s="1">
         <v>45499</v>
       </c>
-      <c r="C16" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="D16">
+      <c r="C16" s="4">
+        <v>0.61458333333333337</v>
+      </c>
+      <c r="D16" s="5">
         <v>4</v>
       </c>
-      <c r="E16" s="2" t="s">
+      <c r="E16" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="1">
         <v>45128</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G16" s="1">
         <v>45132</v>
       </c>
-      <c r="H16">
+      <c r="H16" s="5">
         <v>1</v>
       </c>
-      <c r="I16">
+      <c r="I16" s="5">
         <v>36</v>
       </c>
     </row>
@@ -1027,23 +898,22 @@
       <c r="A17">
         <v>16</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B17" s="1">
         <v>45146</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="D17">
+      <c r="C17" s="4">
+        <v>0.69097222222222221</v>
+      </c>
+      <c r="D17" s="5">
         <v>3</v>
       </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="3">
+      <c r="F17" s="1">
         <v>45147</v>
       </c>
-      <c r="H17">
+      <c r="H17" s="5">
         <v>2</v>
       </c>
-      <c r="I17">
+      <c r="I17" s="5">
         <v>30</v>
       </c>
     </row>
@@ -1051,23 +921,22 @@
       <c r="A18">
         <v>17</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B18" s="1">
         <v>45473</v>
       </c>
-      <c r="C18" s="6" t="s">
-        <v>57</v>
-      </c>
-      <c r="D18">
+      <c r="C18" s="4">
+        <v>0.43055555555555558</v>
+      </c>
+      <c r="D18" s="5">
         <v>1</v>
       </c>
-      <c r="E18" s="2"/>
-      <c r="F18" s="3">
+      <c r="F18" s="1">
         <v>45164</v>
       </c>
-      <c r="H18">
+      <c r="H18" s="5">
         <v>25</v>
       </c>
-      <c r="I18">
+      <c r="I18" s="5">
         <v>29</v>
       </c>
     </row>
@@ -1075,23 +944,22 @@
       <c r="A19">
         <v>18</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B19" s="1">
         <v>45412</v>
       </c>
-      <c r="C19" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D19">
+      <c r="C19" s="4">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="D19" s="5">
         <v>1</v>
       </c>
-      <c r="E19" s="2"/>
-      <c r="F19" s="3">
+      <c r="F19" s="1">
         <v>45146</v>
       </c>
-      <c r="H19">
+      <c r="H19" s="5">
         <v>14</v>
       </c>
-      <c r="I19">
+      <c r="I19" s="5">
         <v>43</v>
       </c>
     </row>
@@ -1099,23 +967,22 @@
       <c r="A20">
         <v>19</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B20" s="1">
         <v>45248</v>
       </c>
-      <c r="C20" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D20">
+      <c r="C20" s="4">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="D20" s="5">
         <v>4</v>
       </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="3">
+      <c r="F20" s="1">
         <v>45156</v>
       </c>
-      <c r="H20">
+      <c r="H20" s="5">
         <v>23</v>
       </c>
-      <c r="I20">
+      <c r="I20" s="5">
         <v>11</v>
       </c>
     </row>
@@ -1123,23 +990,22 @@
       <c r="A21">
         <v>20</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B21" s="1">
         <v>45346</v>
       </c>
-      <c r="C21" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="D21">
+      <c r="C21" s="4">
+        <v>0.85069444444444453</v>
+      </c>
+      <c r="D21" s="5">
         <v>1</v>
       </c>
-      <c r="E21" s="2"/>
-      <c r="F21" s="3">
+      <c r="F21" s="1">
         <v>45125</v>
       </c>
-      <c r="H21">
+      <c r="H21" s="5">
         <v>17</v>
       </c>
-      <c r="I21">
+      <c r="I21" s="5">
         <v>24</v>
       </c>
     </row>
@@ -1147,25 +1013,25 @@
       <c r="A22">
         <v>21</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B22" s="1">
         <v>45347</v>
       </c>
-      <c r="C22" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D22">
+      <c r="C22" s="4">
+        <v>0.57291666666666663</v>
+      </c>
+      <c r="D22" s="5">
         <v>8</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="E22" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F22" s="3">
+      <c r="F22" s="1">
         <v>45140</v>
       </c>
-      <c r="H22">
+      <c r="H22" s="5">
         <v>28</v>
       </c>
-      <c r="I22">
+      <c r="I22" s="5">
         <v>47</v>
       </c>
     </row>
@@ -1173,23 +1039,22 @@
       <c r="A23">
         <v>22</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B23" s="1">
         <v>45406</v>
       </c>
-      <c r="C23" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="D23">
+      <c r="C23" s="4">
+        <v>0.75694444444444453</v>
+      </c>
+      <c r="D23" s="5">
         <v>2</v>
       </c>
-      <c r="E23" s="2"/>
-      <c r="F23" s="3">
+      <c r="F23" s="1">
         <v>45147</v>
       </c>
-      <c r="H23">
+      <c r="H23" s="5">
         <v>21</v>
       </c>
-      <c r="I23">
+      <c r="I23" s="5">
         <v>27</v>
       </c>
     </row>
@@ -1197,23 +1062,22 @@
       <c r="A24">
         <v>23</v>
       </c>
-      <c r="B24" s="3">
+      <c r="B24" s="1">
         <v>45387</v>
       </c>
-      <c r="C24" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="D24">
+      <c r="C24" s="4">
+        <v>0.48958333333333331</v>
+      </c>
+      <c r="D24" s="5">
         <v>9</v>
       </c>
-      <c r="E24" s="2"/>
-      <c r="F24" s="3">
+      <c r="F24" s="1">
         <v>45141</v>
       </c>
-      <c r="H24">
+      <c r="H24" s="5">
         <v>24</v>
       </c>
-      <c r="I24">
+      <c r="I24" s="5">
         <v>34</v>
       </c>
     </row>
@@ -1221,25 +1085,25 @@
       <c r="A25">
         <v>24</v>
       </c>
-      <c r="B25" s="3">
+      <c r="B25" s="1">
         <v>45384</v>
       </c>
-      <c r="C25" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="D25">
+      <c r="C25" s="4">
+        <v>0.76041666666666663</v>
+      </c>
+      <c r="D25" s="5">
         <v>9</v>
       </c>
-      <c r="E25" s="2" t="s">
+      <c r="E25" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F25" s="3">
+      <c r="F25" s="1">
         <v>45154</v>
       </c>
-      <c r="H25">
+      <c r="H25" s="5">
         <v>1</v>
       </c>
-      <c r="I25">
+      <c r="I25" s="5">
         <v>43</v>
       </c>
     </row>
@@ -1247,23 +1111,22 @@
       <c r="A26">
         <v>25</v>
       </c>
-      <c r="B26" s="3">
+      <c r="B26" s="1">
         <v>45301</v>
       </c>
-      <c r="C26" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D26">
+      <c r="C26" s="4">
+        <v>0.79166666666666663</v>
+      </c>
+      <c r="D26" s="5">
         <v>6</v>
       </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="3">
+      <c r="F26" s="1">
         <v>45129</v>
       </c>
-      <c r="H26">
+      <c r="H26" s="5">
         <v>8</v>
       </c>
-      <c r="I26">
+      <c r="I26" s="5">
         <v>31</v>
       </c>
     </row>
@@ -1271,23 +1134,22 @@
       <c r="A27">
         <v>26</v>
       </c>
-      <c r="B27" s="3">
+      <c r="B27" s="1">
         <v>45282</v>
       </c>
-      <c r="C27" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D27">
+      <c r="C27" s="4">
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="D27" s="5">
         <v>3</v>
       </c>
-      <c r="E27" s="2"/>
-      <c r="F27" s="3">
+      <c r="F27" s="1">
         <v>45161</v>
       </c>
-      <c r="H27">
+      <c r="H27" s="5">
         <v>4</v>
       </c>
-      <c r="I27">
+      <c r="I27" s="5">
         <v>7</v>
       </c>
     </row>
@@ -1295,25 +1157,25 @@
       <c r="A28">
         <v>27</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B28" s="1">
         <v>45286</v>
       </c>
-      <c r="C28" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D28">
+      <c r="C28" s="4">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="D28" s="5">
         <v>3</v>
       </c>
-      <c r="E28" s="2" t="s">
+      <c r="E28" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="F28" s="3">
+      <c r="F28" s="1">
         <v>45136</v>
       </c>
-      <c r="H28">
+      <c r="H28" s="5">
         <v>18</v>
       </c>
-      <c r="I28">
+      <c r="I28" s="5">
         <v>3</v>
       </c>
     </row>
@@ -1321,23 +1183,22 @@
       <c r="A29">
         <v>28</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B29" s="1">
         <v>45176</v>
       </c>
-      <c r="C29" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D29">
+      <c r="C29" s="4">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="D29" s="5">
         <v>1</v>
       </c>
-      <c r="E29" s="2"/>
-      <c r="F29" s="3">
+      <c r="F29" s="1">
         <v>45147</v>
       </c>
-      <c r="H29">
+      <c r="H29" s="5">
         <v>23</v>
       </c>
-      <c r="I29">
+      <c r="I29" s="5">
         <v>45</v>
       </c>
     </row>
@@ -1345,25 +1206,25 @@
       <c r="A30">
         <v>29</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B30" s="1">
         <v>45466</v>
       </c>
-      <c r="C30" s="6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D30">
+      <c r="C30" s="4">
+        <v>0.81597222222222221</v>
+      </c>
+      <c r="D30" s="5">
         <v>7</v>
       </c>
-      <c r="E30" s="2" t="s">
+      <c r="E30" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="F30" s="3">
+      <c r="F30" s="1">
         <v>45139</v>
       </c>
-      <c r="H30">
+      <c r="H30" s="5">
         <v>14</v>
       </c>
-      <c r="I30">
+      <c r="I30" s="5">
         <v>15</v>
       </c>
     </row>
@@ -1371,23 +1232,22 @@
       <c r="A31">
         <v>30</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B31" s="1">
         <v>45397</v>
       </c>
-      <c r="C31" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="D31">
+      <c r="C31" s="4">
+        <v>0.62847222222222221</v>
+      </c>
+      <c r="D31" s="5">
         <v>4</v>
       </c>
-      <c r="E31" s="2"/>
-      <c r="F31" s="3">
+      <c r="F31" s="1">
         <v>45147</v>
       </c>
-      <c r="H31">
+      <c r="H31" s="5">
         <v>3</v>
       </c>
-      <c r="I31">
+      <c r="I31" s="5">
         <v>43</v>
       </c>
     </row>
@@ -1395,23 +1255,22 @@
       <c r="A32">
         <v>31</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B32" s="1">
         <v>45261</v>
       </c>
-      <c r="C32" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="D32">
+      <c r="C32" s="4">
+        <v>0.57986111111111105</v>
+      </c>
+      <c r="D32" s="5">
         <v>1</v>
       </c>
-      <c r="E32" s="2"/>
-      <c r="F32" s="3">
+      <c r="F32" s="1">
         <v>45094</v>
       </c>
-      <c r="H32">
+      <c r="H32" s="5">
         <v>11</v>
       </c>
-      <c r="I32">
+      <c r="I32" s="5">
         <v>36</v>
       </c>
     </row>
@@ -1419,23 +1278,22 @@
       <c r="A33">
         <v>32</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B33" s="1">
         <v>45368</v>
       </c>
-      <c r="C33" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="D33">
+      <c r="C33" s="4">
+        <v>0.52083333333333337</v>
+      </c>
+      <c r="D33" s="5">
         <v>8</v>
       </c>
-      <c r="E33" s="2"/>
-      <c r="F33" s="3">
+      <c r="F33" s="1">
         <v>45159</v>
       </c>
-      <c r="H33">
+      <c r="H33" s="5">
         <v>14</v>
       </c>
-      <c r="I33">
+      <c r="I33" s="5">
         <v>6</v>
       </c>
     </row>
@@ -1443,25 +1301,25 @@
       <c r="A34">
         <v>33</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B34" s="1">
         <v>45173</v>
       </c>
-      <c r="C34" s="6" t="s">
-        <v>47</v>
-      </c>
-      <c r="D34">
+      <c r="C34" s="4">
+        <v>0.60763888888888895</v>
+      </c>
+      <c r="D34" s="5">
         <v>6</v>
       </c>
-      <c r="E34" s="2" t="s">
+      <c r="E34" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="F34" s="3">
+      <c r="F34" s="1">
         <v>45147</v>
       </c>
-      <c r="H34">
+      <c r="H34" s="5">
         <v>7</v>
       </c>
-      <c r="I34">
+      <c r="I34" s="5">
         <v>1</v>
       </c>
     </row>
@@ -1469,26 +1327,25 @@
       <c r="A35">
         <v>34</v>
       </c>
-      <c r="B35" s="3">
+      <c r="B35" s="1">
         <v>45287</v>
       </c>
-      <c r="C35" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D35">
+      <c r="C35" s="4">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="D35" s="5">
         <v>2</v>
       </c>
-      <c r="E35" s="2"/>
-      <c r="F35" s="3">
+      <c r="F35" s="1">
         <v>45069</v>
       </c>
-      <c r="G35" s="3">
+      <c r="G35" s="1">
         <v>45120</v>
       </c>
-      <c r="H35">
+      <c r="H35" s="5">
         <v>29</v>
       </c>
-      <c r="I35">
+      <c r="I35" s="5">
         <v>11</v>
       </c>
     </row>
@@ -1496,23 +1353,22 @@
       <c r="A36">
         <v>35</v>
       </c>
-      <c r="B36" s="3">
+      <c r="B36" s="1">
         <v>45486</v>
       </c>
-      <c r="C36" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D36">
+      <c r="C36" s="4">
+        <v>0.375</v>
+      </c>
+      <c r="D36" s="5">
         <v>2</v>
       </c>
-      <c r="E36" s="2"/>
-      <c r="F36" s="3">
+      <c r="F36" s="1">
         <v>45146</v>
       </c>
-      <c r="H36">
+      <c r="H36" s="5">
         <v>25</v>
       </c>
-      <c r="I36">
+      <c r="I36" s="5">
         <v>3</v>
       </c>
     </row>
@@ -1520,23 +1376,22 @@
       <c r="A37">
         <v>36</v>
       </c>
-      <c r="B37" s="3">
+      <c r="B37" s="1">
         <v>45413</v>
       </c>
-      <c r="C37" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="D37">
+      <c r="C37" s="4">
+        <v>0.44097222222222227</v>
+      </c>
+      <c r="D37" s="5">
         <v>3</v>
       </c>
-      <c r="E37" s="2"/>
-      <c r="F37" s="3">
+      <c r="F37" s="1">
         <v>45135</v>
       </c>
-      <c r="H37">
+      <c r="H37" s="5">
         <v>24</v>
       </c>
-      <c r="I37">
+      <c r="I37" s="5">
         <v>4</v>
       </c>
     </row>
@@ -1544,23 +1399,22 @@
       <c r="A38">
         <v>37</v>
       </c>
-      <c r="B38" s="3">
+      <c r="B38" s="1">
         <v>45504</v>
       </c>
-      <c r="C38" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D38">
+      <c r="C38" s="4">
+        <v>0.72916666666666663</v>
+      </c>
+      <c r="D38" s="5">
         <v>5</v>
       </c>
-      <c r="E38" s="2"/>
-      <c r="F38" s="3">
+      <c r="F38" s="1">
         <v>45142</v>
       </c>
-      <c r="H38">
+      <c r="H38" s="5">
         <v>13</v>
       </c>
-      <c r="I38">
+      <c r="I38" s="5">
         <v>7</v>
       </c>
     </row>
@@ -1568,23 +1422,22 @@
       <c r="A39">
         <v>38</v>
       </c>
-      <c r="B39" s="3">
+      <c r="B39" s="1">
         <v>45485</v>
       </c>
-      <c r="C39" s="6" t="s">
-        <v>53</v>
-      </c>
-      <c r="D39">
+      <c r="C39" s="4">
+        <v>0.78125</v>
+      </c>
+      <c r="D39" s="5">
         <v>2</v>
       </c>
-      <c r="E39" s="2"/>
-      <c r="F39" s="3">
+      <c r="F39" s="1">
         <v>45163</v>
       </c>
-      <c r="H39">
+      <c r="H39" s="5">
         <v>25</v>
       </c>
-      <c r="I39">
+      <c r="I39" s="5">
         <v>18</v>
       </c>
     </row>
@@ -1592,25 +1445,25 @@
       <c r="A40">
         <v>39</v>
       </c>
-      <c r="B40" s="3">
+      <c r="B40" s="1">
         <v>45372</v>
       </c>
-      <c r="C40" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D40">
+      <c r="C40" s="4">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="D40" s="5">
         <v>5</v>
       </c>
-      <c r="E40" s="2" t="s">
+      <c r="E40" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F40" s="3">
+      <c r="F40" s="1">
         <v>45147</v>
       </c>
-      <c r="H40">
+      <c r="H40" s="5">
         <v>29</v>
       </c>
-      <c r="I40">
+      <c r="I40" s="5">
         <v>8</v>
       </c>
     </row>
@@ -1618,23 +1471,22 @@
       <c r="A41">
         <v>40</v>
       </c>
-      <c r="B41" s="3">
+      <c r="B41" s="1">
         <v>45170</v>
       </c>
-      <c r="C41" s="6" t="s">
-        <v>54</v>
-      </c>
-      <c r="D41">
+      <c r="C41" s="4">
+        <v>0.63888888888888895</v>
+      </c>
+      <c r="D41" s="5">
         <v>3</v>
       </c>
-      <c r="E41" s="2"/>
-      <c r="F41" s="3">
+      <c r="F41" s="1">
         <v>45147</v>
       </c>
-      <c r="H41">
+      <c r="H41" s="5">
         <v>20</v>
       </c>
-      <c r="I41">
+      <c r="I41" s="5">
         <v>43</v>
       </c>
     </row>
@@ -1642,23 +1494,22 @@
       <c r="A42">
         <v>41</v>
       </c>
-      <c r="B42" s="3">
+      <c r="B42" s="1">
         <v>45192</v>
       </c>
-      <c r="C42" s="6" t="s">
-        <v>58</v>
-      </c>
-      <c r="D42">
+      <c r="C42" s="4">
+        <v>0.75</v>
+      </c>
+      <c r="D42" s="5">
         <v>6</v>
       </c>
-      <c r="E42" s="2"/>
-      <c r="F42" s="3">
+      <c r="F42" s="1">
         <v>45159</v>
       </c>
-      <c r="H42">
+      <c r="H42" s="5">
         <v>16</v>
       </c>
-      <c r="I42">
+      <c r="I42" s="5">
         <v>8</v>
       </c>
     </row>
@@ -1666,25 +1517,25 @@
       <c r="A43">
         <v>42</v>
       </c>
-      <c r="B43" s="3">
+      <c r="B43" s="1">
         <v>45439</v>
       </c>
-      <c r="C43" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D43">
+      <c r="C43" s="4">
+        <v>0.73958333333333337</v>
+      </c>
+      <c r="D43" s="5">
         <v>5</v>
       </c>
-      <c r="E43" s="2" t="s">
+      <c r="E43" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="F43" s="3">
+      <c r="F43" s="1">
         <v>45140</v>
       </c>
-      <c r="H43">
+      <c r="H43" s="5">
         <v>10</v>
       </c>
-      <c r="I43">
+      <c r="I43" s="5">
         <v>18</v>
       </c>
     </row>
@@ -1692,23 +1543,22 @@
       <c r="A44">
         <v>43</v>
       </c>
-      <c r="B44" s="3">
+      <c r="B44" s="1">
         <v>45355</v>
       </c>
-      <c r="C44" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D44">
+      <c r="C44" s="4">
+        <v>0.63541666666666663</v>
+      </c>
+      <c r="D44" s="5">
         <v>3</v>
       </c>
-      <c r="E44" s="2"/>
-      <c r="F44" s="3">
+      <c r="F44" s="1">
         <v>45151</v>
       </c>
-      <c r="H44">
+      <c r="H44" s="5">
         <v>18</v>
       </c>
-      <c r="I44">
+      <c r="I44" s="5">
         <v>20</v>
       </c>
     </row>
@@ -1716,23 +1566,22 @@
       <c r="A45">
         <v>44</v>
       </c>
-      <c r="B45" s="3">
+      <c r="B45" s="1">
         <v>45290</v>
       </c>
-      <c r="C45" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="D45">
+      <c r="C45" s="4">
+        <v>0.625</v>
+      </c>
+      <c r="D45" s="5">
         <v>1</v>
       </c>
-      <c r="E45" s="2"/>
-      <c r="F45" s="3">
+      <c r="F45" s="1">
         <v>45113</v>
       </c>
-      <c r="H45">
+      <c r="H45" s="5">
         <v>8</v>
       </c>
-      <c r="I45">
+      <c r="I45" s="5">
         <v>38</v>
       </c>
     </row>
@@ -1740,23 +1589,22 @@
       <c r="A46">
         <v>45</v>
       </c>
-      <c r="B46" s="3">
+      <c r="B46" s="1">
         <v>45448</v>
       </c>
-      <c r="C46" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="D46">
+      <c r="C46" s="4">
+        <v>0.51041666666666663</v>
+      </c>
+      <c r="D46" s="5">
         <v>6</v>
       </c>
-      <c r="E46" s="2"/>
-      <c r="F46" s="3">
+      <c r="F46" s="1">
         <v>45147</v>
       </c>
-      <c r="H46">
+      <c r="H46" s="5">
         <v>22</v>
       </c>
-      <c r="I46">
+      <c r="I46" s="5">
         <v>27</v>
       </c>
     </row>
@@ -1764,25 +1612,25 @@
       <c r="A47">
         <v>46</v>
       </c>
-      <c r="B47" s="3">
+      <c r="B47" s="1">
         <v>45362</v>
       </c>
-      <c r="C47" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D47">
+      <c r="C47" s="4">
+        <v>0.47916666666666669</v>
+      </c>
+      <c r="D47" s="5">
         <v>4</v>
       </c>
-      <c r="E47" s="2" t="s">
+      <c r="E47" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F47" s="3">
+      <c r="F47" s="1">
         <v>45117</v>
       </c>
-      <c r="H47">
+      <c r="H47" s="5">
         <v>25</v>
       </c>
-      <c r="I47">
+      <c r="I47" s="5">
         <v>25</v>
       </c>
     </row>
@@ -1790,23 +1638,22 @@
       <c r="A48">
         <v>47</v>
       </c>
-      <c r="B48" s="3">
+      <c r="B48" s="1">
         <v>45408</v>
       </c>
-      <c r="C48" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="D48">
+      <c r="C48" s="4">
+        <v>0.69791666666666663</v>
+      </c>
+      <c r="D48" s="5">
         <v>2</v>
       </c>
-      <c r="E48" s="2"/>
-      <c r="F48" s="3">
+      <c r="F48" s="1">
         <v>45164</v>
       </c>
-      <c r="H48">
+      <c r="H48" s="5">
         <v>25</v>
       </c>
-      <c r="I48">
+      <c r="I48" s="5">
         <v>25</v>
       </c>
     </row>
@@ -1814,25 +1661,25 @@
       <c r="A49">
         <v>48</v>
       </c>
-      <c r="B49" s="3">
+      <c r="B49" s="1">
         <v>45275</v>
       </c>
-      <c r="C49" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="D49">
+      <c r="C49" s="4">
+        <v>0.58333333333333337</v>
+      </c>
+      <c r="D49" s="5">
         <v>3</v>
       </c>
-      <c r="E49" s="2" t="s">
+      <c r="E49" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="F49" s="3">
+      <c r="F49" s="1">
         <v>45143</v>
       </c>
-      <c r="H49">
+      <c r="H49" s="5">
         <v>21</v>
       </c>
-      <c r="I49">
+      <c r="I49" s="5">
         <v>40</v>
       </c>
     </row>
@@ -1840,26 +1687,25 @@
       <c r="A50">
         <v>49</v>
       </c>
-      <c r="B50" s="3">
+      <c r="B50" s="1">
         <v>45191</v>
       </c>
-      <c r="C50" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D50">
+      <c r="C50" s="4">
+        <v>0.88541666666666663</v>
+      </c>
+      <c r="D50" s="5">
         <v>2</v>
       </c>
-      <c r="E50" s="2"/>
-      <c r="F50" s="3">
+      <c r="F50" s="1">
         <v>45093</v>
       </c>
-      <c r="G50" s="3">
+      <c r="G50" s="1">
         <v>45133</v>
       </c>
-      <c r="H50">
+      <c r="H50" s="5">
         <v>26</v>
       </c>
-      <c r="I50">
+      <c r="I50" s="5">
         <v>2</v>
       </c>
     </row>
@@ -1867,30 +1713,27 @@
       <c r="A51">
         <v>50</v>
       </c>
-      <c r="B51" s="3">
+      <c r="B51" s="1">
         <v>45462</v>
       </c>
-      <c r="C51" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D51">
+      <c r="C51" s="4">
+        <v>0.46875</v>
+      </c>
+      <c r="D51" s="5">
         <v>4</v>
       </c>
-      <c r="E51" s="2" t="s">
+      <c r="E51" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="F51" s="3">
+      <c r="F51" s="1">
         <v>45149</v>
       </c>
-      <c r="H51">
+      <c r="H51" s="5">
         <v>14</v>
       </c>
-      <c r="I51">
+      <c r="I51" s="5">
         <v>5</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.55000000000000004">
-      <c r="E52" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>